<commit_message>
yearly dates now too
</commit_message>
<xml_diff>
--- a/subset_test_madeup.xlsx
+++ b/subset_test_madeup.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/64_mac/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA153E9-71AB-8D42-9026-56940B80ECCF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CCE428EA-65DF-5C48-9FBE-579B86C74150}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{3A0F1AC4-9379-9848-98EF-ED9504BFDD38}"/>
+    <workbookView xWindow="-4660" yWindow="-18580" windowWidth="25440" windowHeight="15000" xr2:uid="{3A0F1AC4-9379-9848-98EF-ED9504BFDD38}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="subset_test_madeup" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="WIWA_filtered" localSheetId="0">Sheet1!$A$1:$F$669178</definedName>
+    <definedName name="WIWA_filtered" localSheetId="0">subset_test_madeup!$A$1:$F$669178</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -497,7 +497,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -547,7 +547,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="1">
-        <v>39102</v>
+        <v>36911</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -567,7 +567,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="1">
-        <v>39084</v>
+        <v>37258</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -587,7 +587,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="1">
-        <v>39085</v>
+        <v>37624</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -607,7 +607,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1">
-        <v>39086</v>
+        <v>37990</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -627,7 +627,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="1">
-        <v>39087</v>
+        <v>38357</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -647,7 +647,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="1">
-        <v>39114</v>
+        <v>36923</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -667,7 +667,7 @@
         <v>11</v>
       </c>
       <c r="F8" s="1">
-        <v>39115</v>
+        <v>37289</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -687,7 +687,7 @@
         <v>11</v>
       </c>
       <c r="F9" s="1">
-        <v>39116</v>
+        <v>37655</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -707,7 +707,7 @@
         <v>11</v>
       </c>
       <c r="F10" s="1">
-        <v>39117</v>
+        <v>38021</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -727,7 +727,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="1">
-        <v>39142</v>
+        <v>36951</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -747,7 +747,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="1">
-        <v>39143</v>
+        <v>37317</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -767,7 +767,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="1">
-        <v>39144</v>
+        <v>37683</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -787,7 +787,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="1">
-        <v>39145</v>
+        <v>37684</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -807,7 +807,7 @@
         <v>12</v>
       </c>
       <c r="F15" s="1">
-        <v>39146</v>
+        <v>37685</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -827,7 +827,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="1">
-        <v>39147</v>
+        <v>38052</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -847,7 +847,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="1">
-        <v>39148</v>
+        <v>38418</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -867,7 +867,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="1">
-        <v>39173</v>
+        <v>37347</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -887,7 +887,7 @@
         <v>11</v>
       </c>
       <c r="F19" s="1">
-        <v>39174</v>
+        <v>37348</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -907,7 +907,7 @@
         <v>11</v>
       </c>
       <c r="F20" s="1">
-        <v>39175</v>
+        <v>39541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>